<commit_message>
add two tabs for grid-view of releases and provide publication information
</commit_message>
<xml_diff>
--- a/Stats Publication Leads.xlsx
+++ b/Stats Publication Leads.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://justiceuk-my.sharepoint.com/personal/hayden_smith_justice_gov_uk/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="131" documentId="8_{5D22F1CC-6B7E-4D6D-965B-C445E9D76E27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F1965B93-BFD8-4CE7-9CAA-EB9C0B9808B3}"/>
+  <xr:revisionPtr revIDLastSave="132" documentId="8_{5D22F1CC-6B7E-4D6D-965B-C445E9D76E27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DEF01D18-ED7D-4476-86EF-042AA4E77904}"/>
   <bookViews>
     <workbookView xWindow="-3732" yWindow="-17388" windowWidth="30936" windowHeight="16776" xr2:uid="{D9DAD797-3196-47A8-927E-B65CA5FE599E}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="174">
   <si>
     <t>Title</t>
   </si>
@@ -563,6 +563,9 @@
   </si>
   <si>
     <t>Laura Davis</t>
+  </si>
+  <si>
+    <t>Justice data lab statistics</t>
   </si>
 </sst>
 </file>
@@ -1483,7 +1486,7 @@
       <selection activeCell="A2" sqref="A2"/>
       <selection pane="topRight" activeCell="A2" sqref="A2"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D23" sqref="D23"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1527,7 +1530,9 @@
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>173</v>
+      </c>
       <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
@@ -2459,15 +2464,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BFA604A9C3983C42BD25AD6B677D13E2" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0b7b66054bf514abfae6322c23004b28">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3d62609a-7e30-44b8-a432-cdf7356e24ea" xmlns:ns3="351d582a-7b6f-46d7-8ce9-09297641bd46" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="791102654b535ba2954fb47e85e2201c" ns2:_="" ns3:_="">
     <xsd:import namespace="3d62609a-7e30-44b8-a432-cdf7356e24ea"/>
@@ -2696,6 +2692,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{604A6221-C1B2-41C8-8D4F-4E88F9B37FB1}">
   <ds:schemaRefs>
@@ -2714,14 +2719,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11924491-05F8-4976-B631-407825EBE43A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A97A81B0-2DF2-468B-B6AD-3D7D9D3DB556}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2738,4 +2735,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11924491-05F8-4976-B631-407825EBE43A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add 'confirm release date by' column
</commit_message>
<xml_diff>
--- a/Stats Publication Leads.xlsx
+++ b/Stats Publication Leads.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://justiceuk-my.sharepoint.com/personal/hayden_smith_justice_gov_uk/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="198" documentId="8_{5D22F1CC-6B7E-4D6D-965B-C445E9D76E27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2EDEA323-14F2-49FC-BCEB-860DCBBC89ED}"/>
+  <xr:revisionPtr revIDLastSave="199" documentId="8_{5D22F1CC-6B7E-4D6D-965B-C445E9D76E27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7181A4E1-80C7-4A6F-85B5-AAB7F7DFA366}"/>
   <bookViews>
-    <workbookView xWindow="-3732" yWindow="-17388" windowWidth="30936" windowHeight="16776" xr2:uid="{D9DAD797-3196-47A8-927E-B65CA5FE599E}"/>
+    <workbookView xWindow="-3840" yWindow="-17388" windowWidth="30936" windowHeight="16776" xr2:uid="{D9DAD797-3196-47A8-927E-B65CA5FE599E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -457,9 +457,6 @@
     <t>long_title</t>
   </si>
   <si>
-    <t>Civil justice statistics</t>
-  </si>
-  <si>
     <t>Prison Population Projections</t>
   </si>
   <si>
@@ -665,6 +662,9 @@
   </si>
   <si>
     <t>Serious further offences</t>
+  </si>
+  <si>
+    <t>Civil justice statistics quarterly</t>
   </si>
 </sst>
 </file>
@@ -1581,11 +1581,11 @@
   <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
       <selection pane="topRight" activeCell="A2" sqref="A2"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B29" sqref="B29"/>
+      <selection pane="bottomRight" activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1608,7 +1608,7 @@
         <v>136</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>1</v>
@@ -1626,7 +1626,7 @@
         <v>5</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -1634,10 +1634,10 @@
         <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>7</v>
@@ -1655,7 +1655,7 @@
         <v>11</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -1666,7 +1666,7 @@
         <v>135</v>
       </c>
       <c r="C3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>7</v>
@@ -1684,7 +1684,7 @@
         <v>15</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="72" x14ac:dyDescent="0.3">
@@ -1695,7 +1695,7 @@
         <v>111</v>
       </c>
       <c r="C4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>7</v>
@@ -1713,7 +1713,7 @@
         <v>15</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -1724,7 +1724,7 @@
         <v>129</v>
       </c>
       <c r="C5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>7</v>
@@ -1742,7 +1742,7 @@
         <v>15</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -1753,7 +1753,7 @@
         <v>115</v>
       </c>
       <c r="C6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>7</v>
@@ -1771,7 +1771,7 @@
         <v>15</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -1782,7 +1782,7 @@
         <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>28</v>
@@ -1800,7 +1800,7 @@
         <v>11</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -1811,7 +1811,7 @@
         <v>116</v>
       </c>
       <c r="C8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>32</v>
@@ -1823,13 +1823,13 @@
         <v>34</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H8" s="5" t="s">
         <v>15</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -1840,25 +1840,25 @@
         <v>117</v>
       </c>
       <c r="C9" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>32</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>36</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H9" s="5" t="s">
         <v>15</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
@@ -1866,10 +1866,10 @@
         <v>37</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C10" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>32</v>
@@ -1896,7 +1896,7 @@
         <v>118</v>
       </c>
       <c r="C11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>41</v>
@@ -1914,7 +1914,7 @@
         <v>11</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
@@ -1922,10 +1922,10 @@
         <v>43</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>137</v>
+        <v>206</v>
       </c>
       <c r="C12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>44</v>
@@ -1937,13 +1937,13 @@
         <v>34</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H12" s="5" t="s">
         <v>15</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -1954,7 +1954,7 @@
         <v>119</v>
       </c>
       <c r="C13" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>44</v>
@@ -1966,13 +1966,13 @@
         <v>34</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H13" s="5" t="s">
         <v>15</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
@@ -1983,7 +1983,7 @@
         <v>112</v>
       </c>
       <c r="C14" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>44</v>
@@ -2001,7 +2001,7 @@
         <v>15</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
@@ -2012,7 +2012,7 @@
         <v>113</v>
       </c>
       <c r="C15" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>44</v>
@@ -2030,7 +2030,7 @@
         <v>15</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
@@ -2041,25 +2041,25 @@
         <v>114</v>
       </c>
       <c r="C16" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>44</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>36</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H16" s="5" t="s">
         <v>15</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
@@ -2070,7 +2070,7 @@
         <v>120</v>
       </c>
       <c r="C17" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>55</v>
@@ -2088,7 +2088,7 @@
         <v>11</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
@@ -2099,7 +2099,7 @@
         <v>121</v>
       </c>
       <c r="C18" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>60</v>
@@ -2111,13 +2111,13 @@
         <v>34</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H18" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
@@ -2128,7 +2128,7 @@
         <v>122</v>
       </c>
       <c r="C19" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>62</v>
@@ -2146,7 +2146,7 @@
         <v>15</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
@@ -2154,10 +2154,10 @@
         <v>66</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C20" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>67</v>
@@ -2175,7 +2175,7 @@
         <v>11</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
@@ -2186,7 +2186,7 @@
         <v>123</v>
       </c>
       <c r="C21" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>71</v>
@@ -2204,7 +2204,7 @@
         <v>11</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
@@ -2212,10 +2212,10 @@
         <v>73</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C22" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>74</v>
@@ -2242,7 +2242,7 @@
         <v>124</v>
       </c>
       <c r="C23" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>77</v>
@@ -2256,7 +2256,7 @@
         <v>11</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
@@ -2267,7 +2267,7 @@
         <v>125</v>
       </c>
       <c r="C24" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>77</v>
@@ -2285,7 +2285,7 @@
         <v>11</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
@@ -2296,25 +2296,25 @@
         <v>127</v>
       </c>
       <c r="C25" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>74</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>36</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H25" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
@@ -2325,25 +2325,25 @@
         <v>126</v>
       </c>
       <c r="C26" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>74</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>36</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H26" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
@@ -2351,10 +2351,10 @@
         <v>83</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C27" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>84</v>
@@ -2372,7 +2372,7 @@
         <v>11</v>
       </c>
       <c r="I27" s="6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
@@ -2380,10 +2380,10 @@
         <v>86</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C28" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>77</v>
@@ -2397,7 +2397,7 @@
         <v>15</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
@@ -2408,7 +2408,7 @@
         <v>128</v>
       </c>
       <c r="C29" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>62</v>
@@ -2426,7 +2426,7 @@
         <v>11</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
@@ -2437,7 +2437,7 @@
         <v>130</v>
       </c>
       <c r="C30" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>7</v>
@@ -2455,7 +2455,7 @@
         <v>11</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
@@ -2466,7 +2466,7 @@
         <v>95</v>
       </c>
       <c r="C31" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>96</v>
@@ -2484,7 +2484,7 @@
         <v>11</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
@@ -2495,7 +2495,7 @@
         <v>133</v>
       </c>
       <c r="C32" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>98</v>
@@ -2513,7 +2513,7 @@
         <v>15</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
@@ -2521,10 +2521,10 @@
         <v>99</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C33" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>98</v>
@@ -2542,7 +2542,7 @@
         <v>15</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
@@ -2553,7 +2553,7 @@
         <v>131</v>
       </c>
       <c r="C34" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>98</v>
@@ -2571,7 +2571,7 @@
         <v>15</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
@@ -2582,7 +2582,7 @@
         <v>134</v>
       </c>
       <c r="C35" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>104</v>
@@ -2600,7 +2600,7 @@
         <v>11</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
@@ -2611,7 +2611,7 @@
         <v>132</v>
       </c>
       <c r="C36" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>106</v>
@@ -2629,7 +2629,7 @@
         <v>15</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
@@ -2640,7 +2640,7 @@
         <v>109</v>
       </c>
       <c r="C37" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>110</v>
@@ -2654,7 +2654,7 @@
         <v>15</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -2673,6 +2673,17 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3d62609a-7e30-44b8-a432-cdf7356e24ea">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="351d582a-7b6f-46d7-8ce9-09297641bd46" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BFA604A9C3983C42BD25AD6B677D13E2" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0b7b66054bf514abfae6322c23004b28">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3d62609a-7e30-44b8-a432-cdf7356e24ea" xmlns:ns3="351d582a-7b6f-46d7-8ce9-09297641bd46" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="791102654b535ba2954fb47e85e2201c" ns2:_="" ns3:_="">
     <xsd:import namespace="3d62609a-7e30-44b8-a432-cdf7356e24ea"/>
@@ -2901,17 +2912,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3d62609a-7e30-44b8-a432-cdf7356e24ea">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="351d582a-7b6f-46d7-8ce9-09297641bd46" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11924491-05F8-4976-B631-407825EBE43A}">
   <ds:schemaRefs>
@@ -2921,6 +2921,23 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{604A6221-C1B2-41C8-8D4F-4E88F9B37FB1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="3d62609a-7e30-44b8-a432-cdf7356e24ea"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="351d582a-7b6f-46d7-8ce9-09297641bd46"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A97A81B0-2DF2-468B-B6AD-3D7D9D3DB556}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2937,21 +2954,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{604A6221-C1B2-41C8-8D4F-4E88F9B37FB1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="3d62609a-7e30-44b8-a432-cdf7356e24ea"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="351d582a-7b6f-46d7-8ce9-09297641bd46"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>